<commit_message>
update unit tests to avoid PII scans
Signed-off-by: automike <mikeliucc@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/script/unitTest_expressions_more.xlsx
+++ b/src/test/resources/unittesting/artifact/script/unitTest_expressions_more.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nexial\nexial-core\src\test\resources\unittesting\artifact\script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7756E3A-2F7D-4DAB-BDC3-B71047B43CCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D105A146-5627-47A6-AE3A-B689339A0D5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2167" uniqueCount="1156">
   <si>
     <t>target</t>
   </si>
@@ -3914,40 +3914,6 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">[CSV(${csvData}) =&gt;
- parse(header=true)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="8" tint="-0.249977111117893"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve"> htmlTable
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
-      <t>save($(syspath|data|fullpath)/unitTest_expression_csv04.html,false)
-]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">[CSV(${csvData}) =&gt; parse(header=true) </t>
     </r>
     <r>
@@ -6091,15 +6057,6 @@
 567890123,Jim,Manager,45) =&gt; headers]</t>
   </si>
   <si>
-    <t xml:space="preserve">NUM,Name,WORD,NUM2
-123456789,James,Accountant,41
-234567890,Jim,Educator,42
-345678901,"Johnson, Adam",Inspector General,23
-456789012,Jenny,Cashier,23
-567890123,Jim,Manager,45
-</t>
-  </si>
-  <si>
     <t>NUM,Name,WORD,NUM2
 123456789,James,Accountant,41
 234567890,Jim,Educator,42
@@ -6558,6 +6515,32 @@
 ----------------------------------------------------
 |567890123 |Jon           |Manager           |41   |
 ----------------------------------------------------</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[CSV(${csvData}) =&gt; parse(header=true)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="8" tint="-0.249977111117893"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> htmlTable </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>save($(syspath|out|fullpath)/unitTest_csv.html,false)
+]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -7658,7 +7641,7 @@
         <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="K2" t="s">
         <v>41</v>
@@ -7679,7 +7662,7 @@
         <v>46</v>
       </c>
       <c r="Q2" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="R2" t="s">
         <v>48</v>
@@ -7774,7 +7757,7 @@
         <v>76</v>
       </c>
       <c r="Q3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="R3" t="s">
         <v>77</v>
@@ -7946,7 +7929,7 @@
         <v>127</v>
       </c>
       <c r="Q5" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="R5" t="s">
         <v>128</v>
@@ -8079,7 +8062,7 @@
         <v>166</v>
       </c>
       <c r="L7" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="N7" t="s">
         <v>42</v>
@@ -8285,7 +8268,7 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="H11" t="s">
         <v>227</v>
@@ -8382,7 +8365,7 @@
         <v>253</v>
       </c>
       <c r="S13" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="AA13" t="s">
         <v>255</v>
@@ -8568,7 +8551,7 @@
         <v>298</v>
       </c>
       <c r="S19" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="AA19" t="s">
         <v>306</v>
@@ -8614,7 +8597,7 @@
         <v>310</v>
       </c>
       <c r="S21" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="AA21" t="s">
         <v>316</v>
@@ -12656,10 +12639,10 @@
     </row>
     <row r="116" spans="1:12" ht="21" customHeight="1">
       <c r="A116" s="66" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B116" s="67" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C116" s="69" t="s">
         <v>5</v>
@@ -12668,15 +12651,15 @@
         <v>42</v>
       </c>
       <c r="E116" s="68" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="F116" s="68" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="117" spans="1:12" ht="21" customHeight="1">
       <c r="B117" s="67" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C117" s="69" t="s">
         <v>5</v>
@@ -12685,10 +12668,10 @@
         <v>42</v>
       </c>
       <c r="E117" s="68" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="F117" s="68" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="118" spans="1:12" ht="21" customHeight="1"/>
@@ -15048,10 +15031,10 @@
     </row>
     <row r="88" spans="1:15" ht="90">
       <c r="A88" s="21" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="C88" s="23" t="s">
         <v>5</v>
@@ -15060,10 +15043,10 @@
         <v>42</v>
       </c>
       <c r="E88" s="65" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="F88" s="60" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="G88" s="24"/>
       <c r="H88" s="24"/>
@@ -15157,9 +15140,9 @@
   <dimension ref="A1:O147"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
@@ -15309,7 +15292,7 @@
         <v>896</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
@@ -15331,7 +15314,7 @@
         <v>42</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>897</v>
@@ -15361,7 +15344,7 @@
         <v>896</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
@@ -15413,7 +15396,7 @@
         <v>896</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
@@ -15487,7 +15470,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="F12" s="25" t="s">
         <v>906</v>
@@ -15514,7 +15497,7 @@
         <v>42</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="F13" s="25" t="s">
         <v>907</v>
@@ -15544,7 +15527,7 @@
         <v>896</v>
       </c>
       <c r="F14" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="24"/>
@@ -15566,7 +15549,7 @@
         <v>42</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="F15" s="25" t="s">
         <v>909</v>
@@ -15619,7 +15602,7 @@
         <v>896</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="G17" s="24"/>
       <c r="H17" s="24"/>
@@ -15641,7 +15624,7 @@
         <v>42</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="F18" s="25" t="s">
         <v>911</v>
@@ -15671,7 +15654,7 @@
         <v>896</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G19" s="24"/>
       <c r="H19" s="24"/>
@@ -15771,7 +15754,7 @@
         <v>896</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
@@ -15818,7 +15801,7 @@
         <v>42</v>
       </c>
       <c r="E25" s="25" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F25" s="25" t="s">
         <v>921</v>
@@ -15848,7 +15831,7 @@
         <v>896</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G26" s="24"/>
       <c r="H26" s="24"/>
@@ -15870,10 +15853,10 @@
         <v>42</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="F27" s="25" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
@@ -15895,7 +15878,7 @@
         <v>42</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F28" s="25" t="s">
         <v>923</v>
@@ -16154,7 +16137,7 @@
         <v>896</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
@@ -16176,7 +16159,7 @@
         <v>42</v>
       </c>
       <c r="E39" s="25" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="F39" s="25" t="s">
         <v>939</v>
@@ -16201,7 +16184,7 @@
         <v>42</v>
       </c>
       <c r="E40" s="25" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="F40" s="25" t="s">
         <v>940</v>
@@ -16226,7 +16209,7 @@
         <v>42</v>
       </c>
       <c r="E41" s="25" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="F41" s="25" t="s">
         <v>941</v>
@@ -16256,7 +16239,7 @@
         <v>896</v>
       </c>
       <c r="F42" s="25" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G42" s="24"/>
       <c r="H42" s="24"/>
@@ -16278,10 +16261,10 @@
         <v>42</v>
       </c>
       <c r="E43" s="25" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="F43" s="25" t="s">
-        <v>943</v>
+        <v>1155</v>
       </c>
       <c r="G43" s="25"/>
       <c r="H43" s="24"/>
@@ -16293,7 +16276,7 @@
       <c r="N43" s="19"/>
       <c r="O43" s="18"/>
     </row>
-    <row r="44" spans="1:15" s="2" customFormat="1" ht="105">
+    <row r="44" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A44" s="21" t="s">
         <v>13</v>
       </c>
@@ -16308,7 +16291,7 @@
         <v>896</v>
       </c>
       <c r="F44" s="25" t="s">
-        <v>1098</v>
+        <v>1091</v>
       </c>
       <c r="G44" s="24"/>
       <c r="H44" s="24"/>
@@ -16330,10 +16313,10 @@
         <v>42</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="F45" s="25" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="G45" s="25"/>
       <c r="H45" s="24"/>
@@ -16355,10 +16338,10 @@
         <v>42</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="F46" s="25" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="G46" s="25"/>
       <c r="H46" s="24"/>
@@ -16385,7 +16368,7 @@
         <v>896</v>
       </c>
       <c r="F47" s="25" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G47" s="24"/>
       <c r="H47" s="24"/>
@@ -16410,7 +16393,7 @@
         <v>789</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="G48" s="24"/>
       <c r="H48" s="24"/>
@@ -16432,10 +16415,10 @@
         <v>42</v>
       </c>
       <c r="E49" s="25" t="s">
+        <v>946</v>
+      </c>
+      <c r="F49" s="25" t="s">
         <v>947</v>
-      </c>
-      <c r="F49" s="25" t="s">
-        <v>948</v>
       </c>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
@@ -16449,10 +16432,10 @@
     </row>
     <row r="50" spans="1:15" s="2" customFormat="1" ht="75">
       <c r="A50" s="21" t="s">
+        <v>948</v>
+      </c>
+      <c r="B50" s="22" t="s">
         <v>949</v>
-      </c>
-      <c r="B50" s="22" t="s">
-        <v>950</v>
       </c>
       <c r="C50" s="23" t="s">
         <v>5</v>
@@ -16461,10 +16444,10 @@
         <v>352</v>
       </c>
       <c r="E50" s="24" t="s">
+        <v>950</v>
+      </c>
+      <c r="F50" s="25" t="s">
         <v>951</v>
-      </c>
-      <c r="F50" s="25" t="s">
-        <v>952</v>
       </c>
       <c r="G50" s="24"/>
       <c r="H50" s="24"/>
@@ -16486,10 +16469,10 @@
         <v>352</v>
       </c>
       <c r="E51" s="24" t="s">
+        <v>952</v>
+      </c>
+      <c r="F51" s="25" t="s">
         <v>953</v>
-      </c>
-      <c r="F51" s="25" t="s">
-        <v>954</v>
       </c>
       <c r="G51" s="24"/>
       <c r="H51" s="24"/>
@@ -16511,10 +16494,10 @@
         <v>42</v>
       </c>
       <c r="E52" s="25" t="s">
+        <v>953</v>
+      </c>
+      <c r="F52" s="25" t="s">
         <v>954</v>
-      </c>
-      <c r="F52" s="25" t="s">
-        <v>955</v>
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="24"/>
@@ -16536,10 +16519,10 @@
         <v>42</v>
       </c>
       <c r="E53" s="25" t="s">
+        <v>955</v>
+      </c>
+      <c r="F53" s="25" t="s">
         <v>956</v>
-      </c>
-      <c r="F53" s="25" t="s">
-        <v>957</v>
       </c>
       <c r="G53" s="25"/>
       <c r="H53" s="24"/>
@@ -16554,7 +16537,7 @@
     <row r="54" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A54" s="29"/>
       <c r="B54" s="30" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>5</v>
@@ -16563,10 +16546,10 @@
         <v>352</v>
       </c>
       <c r="E54" s="24" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F54" s="25" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="G54" s="24"/>
       <c r="H54" s="24"/>
@@ -16588,10 +16571,10 @@
         <v>352</v>
       </c>
       <c r="E55" s="24" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F55" s="25" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="G55" s="24"/>
       <c r="H55" s="24"/>
@@ -16613,10 +16596,10 @@
         <v>42</v>
       </c>
       <c r="E56" s="25" t="s">
+        <v>959</v>
+      </c>
+      <c r="F56" s="25" t="s">
         <v>960</v>
-      </c>
-      <c r="F56" s="25" t="s">
-        <v>961</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="24"/>
@@ -16638,10 +16621,10 @@
         <v>42</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="F57" s="25" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="G57" s="24"/>
       <c r="H57" s="24"/>
@@ -16656,7 +16639,7 @@
     <row r="58" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A58" s="21"/>
       <c r="B58" s="22" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C58" s="23" t="s">
         <v>5</v>
@@ -16665,10 +16648,10 @@
         <v>352</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F58" s="25" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="G58" s="24"/>
       <c r="H58" s="24"/>
@@ -16690,10 +16673,10 @@
         <v>352</v>
       </c>
       <c r="E59" s="24" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F59" s="25" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="G59" s="24"/>
       <c r="H59" s="24"/>
@@ -16715,10 +16698,10 @@
         <v>42</v>
       </c>
       <c r="E60" s="25" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="F60" s="25" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G60" s="25"/>
       <c r="H60" s="24"/>
@@ -16740,10 +16723,10 @@
         <v>42</v>
       </c>
       <c r="E61" s="25" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="F61" s="25" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="G61" s="24"/>
       <c r="H61" s="24"/>
@@ -16765,10 +16748,10 @@
         <v>352</v>
       </c>
       <c r="E62" s="25" t="s">
+        <v>962</v>
+      </c>
+      <c r="F62" s="25" t="s">
         <v>963</v>
-      </c>
-      <c r="F62" s="25" t="s">
-        <v>964</v>
       </c>
       <c r="G62" s="24"/>
       <c r="H62" s="24"/>
@@ -16790,7 +16773,7 @@
         <v>394</v>
       </c>
       <c r="E63" s="25" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="F63" s="25"/>
       <c r="G63" s="24"/>
@@ -16813,7 +16796,7 @@
         <v>394</v>
       </c>
       <c r="E64" s="25" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="F64" s="25"/>
       <c r="G64" s="24"/>
@@ -16836,10 +16819,10 @@
         <v>352</v>
       </c>
       <c r="E65" s="25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F65" s="25" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="G65" s="24"/>
       <c r="H65" s="24"/>
@@ -16861,10 +16844,10 @@
         <v>42</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="F66" s="25" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G66" s="24"/>
       <c r="H66" s="24"/>
@@ -16886,7 +16869,7 @@
         <v>394</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="F67" s="25"/>
       <c r="G67" s="24"/>
@@ -16902,7 +16885,7 @@
     <row r="68" spans="1:15" s="2" customFormat="1" ht="60">
       <c r="A68" s="21"/>
       <c r="B68" s="22" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C68" s="23" t="s">
         <v>5</v>
@@ -16911,10 +16894,10 @@
         <v>352</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F68" s="25" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="G68" s="24"/>
       <c r="H68" s="24"/>
@@ -16936,10 +16919,10 @@
         <v>352</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F69" s="25" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="G69" s="24"/>
       <c r="H69" s="24"/>
@@ -16961,7 +16944,7 @@
         <v>394</v>
       </c>
       <c r="E70" s="25" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="F70" s="25"/>
       <c r="G70" s="24"/>
@@ -16984,10 +16967,10 @@
         <v>42</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="F71" s="25" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="G71" s="24"/>
       <c r="H71" s="24"/>
@@ -17009,10 +16992,10 @@
         <v>42</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="F72" s="25" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="G72" s="24"/>
       <c r="H72" s="24"/>
@@ -17026,7 +17009,7 @@
     </row>
     <row r="73" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A73" s="21" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B73" s="22"/>
       <c r="C73" s="23" t="s">
@@ -17039,7 +17022,7 @@
         <v>896</v>
       </c>
       <c r="F73" s="25" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="G73" s="24"/>
       <c r="H73" s="24"/>
@@ -17061,10 +17044,10 @@
         <v>42</v>
       </c>
       <c r="E74" s="25" t="s">
+        <v>969</v>
+      </c>
+      <c r="F74" s="25" t="s">
         <v>970</v>
-      </c>
-      <c r="F74" s="25" t="s">
-        <v>971</v>
       </c>
       <c r="G74" s="25"/>
       <c r="H74" s="24"/>
@@ -17078,7 +17061,7 @@
     </row>
     <row r="75" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A75" s="37" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B75" s="38"/>
       <c r="C75" s="23" t="s">
@@ -17091,7 +17074,7 @@
         <v>896</v>
       </c>
       <c r="F75" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G75" s="24"/>
       <c r="H75" s="24"/>
@@ -17113,10 +17096,10 @@
         <v>42</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="F76" s="25" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="G76" s="25"/>
       <c r="H76" s="24"/>
@@ -17138,10 +17121,10 @@
         <v>42</v>
       </c>
       <c r="E77" s="25" t="s">
+        <v>971</v>
+      </c>
+      <c r="F77" s="25" t="s">
         <v>972</v>
-      </c>
-      <c r="F77" s="25" t="s">
-        <v>973</v>
       </c>
       <c r="G77" s="25"/>
       <c r="H77" s="24"/>
@@ -17155,7 +17138,7 @@
     </row>
     <row r="78" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A78" s="21" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B78" s="22"/>
       <c r="C78" s="23" t="s">
@@ -17168,7 +17151,7 @@
         <v>896</v>
       </c>
       <c r="F78" s="39" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="G78" s="24"/>
       <c r="H78" s="24"/>
@@ -17190,10 +17173,10 @@
         <v>42</v>
       </c>
       <c r="E79" s="25" t="s">
+        <v>975</v>
+      </c>
+      <c r="F79" s="39" t="s">
         <v>976</v>
-      </c>
-      <c r="F79" s="39" t="s">
-        <v>977</v>
       </c>
       <c r="G79" s="25"/>
       <c r="H79" s="24"/>
@@ -17215,10 +17198,10 @@
         <v>42</v>
       </c>
       <c r="E80" s="40" t="s">
+        <v>977</v>
+      </c>
+      <c r="F80" s="25" t="s">
         <v>978</v>
-      </c>
-      <c r="F80" s="25" t="s">
-        <v>979</v>
       </c>
       <c r="G80" s="25"/>
       <c r="H80" s="24"/>
@@ -17240,10 +17223,10 @@
         <v>42</v>
       </c>
       <c r="E81" s="25" t="s">
+        <v>979</v>
+      </c>
+      <c r="F81" s="39" t="s">
         <v>980</v>
-      </c>
-      <c r="F81" s="39" t="s">
-        <v>981</v>
       </c>
       <c r="G81" s="25"/>
       <c r="H81" s="24"/>
@@ -17257,7 +17240,7 @@
     </row>
     <row r="82" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A82" s="37" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B82" s="38"/>
       <c r="C82" s="23" t="s">
@@ -17270,7 +17253,7 @@
         <v>896</v>
       </c>
       <c r="F82" s="25" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G82" s="24"/>
       <c r="H82" s="24"/>
@@ -17292,10 +17275,10 @@
         <v>42</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="F83" s="25" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="G83" s="25"/>
       <c r="H83" s="24"/>
@@ -17309,7 +17292,7 @@
     </row>
     <row r="84" spans="1:15" s="2" customFormat="1" ht="165">
       <c r="A84" s="21" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B84" s="22"/>
       <c r="C84" s="23" t="s">
@@ -17319,10 +17302,10 @@
         <v>42</v>
       </c>
       <c r="E84" s="25" t="s">
+        <v>983</v>
+      </c>
+      <c r="F84" s="25" t="s">
         <v>984</v>
-      </c>
-      <c r="F84" s="25" t="s">
-        <v>985</v>
       </c>
       <c r="G84" s="25"/>
       <c r="H84" s="24"/>
@@ -17336,7 +17319,7 @@
     </row>
     <row r="85" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A85" s="41" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="B85" s="38"/>
       <c r="C85" s="23" t="s">
@@ -17349,7 +17332,7 @@
         <v>896</v>
       </c>
       <c r="F85" s="25" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="G85" s="24"/>
       <c r="H85" s="24"/>
@@ -17364,7 +17347,7 @@
     <row r="86" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A86" s="21"/>
       <c r="B86" s="22" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C86" s="23" t="s">
         <v>5</v>
@@ -17373,10 +17356,10 @@
         <v>42</v>
       </c>
       <c r="E86" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="F86" s="25" t="s">
         <v>989</v>
-      </c>
-      <c r="F86" s="25" t="s">
-        <v>990</v>
       </c>
       <c r="G86" s="25"/>
       <c r="H86" s="24"/>
@@ -17391,7 +17374,7 @@
     <row r="87" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A87" s="21"/>
       <c r="B87" s="22" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C87" s="23" t="s">
         <v>5</v>
@@ -17400,10 +17383,10 @@
         <v>42</v>
       </c>
       <c r="E87" s="25" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F87" s="25" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="G87" s="25"/>
       <c r="H87" s="24"/>
@@ -17418,7 +17401,7 @@
     <row r="88" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A88" s="21"/>
       <c r="B88" s="22" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C88" s="23" t="s">
         <v>5</v>
@@ -17427,10 +17410,10 @@
         <v>42</v>
       </c>
       <c r="E88" s="25" t="s">
+        <v>993</v>
+      </c>
+      <c r="F88" s="25" t="s">
         <v>994</v>
-      </c>
-      <c r="F88" s="25" t="s">
-        <v>995</v>
       </c>
       <c r="G88" s="25"/>
       <c r="H88" s="24"/>
@@ -17452,10 +17435,10 @@
         <v>42</v>
       </c>
       <c r="E89" s="25" t="s">
+        <v>995</v>
+      </c>
+      <c r="F89" s="25" t="s">
         <v>996</v>
-      </c>
-      <c r="F89" s="25" t="s">
-        <v>997</v>
       </c>
       <c r="G89" s="25"/>
       <c r="H89" s="24"/>
@@ -17469,7 +17452,7 @@
     </row>
     <row r="90" spans="1:15" s="2" customFormat="1" ht="105">
       <c r="A90" s="21" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B90" s="22"/>
       <c r="C90" s="23" t="s">
@@ -17482,7 +17465,7 @@
         <v>896</v>
       </c>
       <c r="F90" s="25" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="G90" s="24"/>
       <c r="H90" s="24"/>
@@ -17497,7 +17480,7 @@
     <row r="91" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A91" s="21"/>
       <c r="B91" s="22" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C91" s="23" t="s">
         <v>5</v>
@@ -17506,10 +17489,10 @@
         <v>42</v>
       </c>
       <c r="E91" s="25" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F91" s="25" t="s">
         <v>1131</v>
-      </c>
-      <c r="F91" s="25" t="s">
-        <v>1133</v>
       </c>
       <c r="G91" s="25"/>
       <c r="H91" s="24"/>
@@ -17533,10 +17516,10 @@
         <v>42</v>
       </c>
       <c r="E92" s="25" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="F92" s="25" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="G92" s="6"/>
       <c r="H92" s="24"/>
@@ -17551,7 +17534,7 @@
     <row r="93" spans="1:15" s="2" customFormat="1" ht="105">
       <c r="A93" s="21"/>
       <c r="B93" s="22" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C93" s="23" t="s">
         <v>5</v>
@@ -17560,10 +17543,10 @@
         <v>42</v>
       </c>
       <c r="E93" s="25" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="F93" s="25" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="G93" s="25"/>
       <c r="H93" s="24"/>
@@ -17577,7 +17560,7 @@
     </row>
     <row r="94" spans="1:15" s="2" customFormat="1" ht="105">
       <c r="A94" s="21" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B94" s="22"/>
       <c r="C94" s="23" t="s">
@@ -17590,7 +17573,7 @@
         <v>896</v>
       </c>
       <c r="F94" s="25" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="G94" s="25"/>
       <c r="H94" s="24"/>
@@ -17612,10 +17595,10 @@
         <v>42</v>
       </c>
       <c r="E95" s="25" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F95" s="25" t="s">
         <v>1004</v>
-      </c>
-      <c r="F95" s="25" t="s">
-        <v>1005</v>
       </c>
       <c r="G95" s="25"/>
       <c r="H95" s="24"/>
@@ -17629,7 +17612,7 @@
     </row>
     <row r="96" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A96" s="21" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B96" s="22"/>
       <c r="C96" s="23" t="s">
@@ -17642,7 +17625,7 @@
         <v>896</v>
       </c>
       <c r="F96" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G96" s="24"/>
       <c r="H96" s="24"/>
@@ -17667,7 +17650,7 @@
         <v>789</v>
       </c>
       <c r="F97" s="25" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="G97" s="24"/>
       <c r="H97" s="24"/>
@@ -17694,7 +17677,7 @@
         <v>896</v>
       </c>
       <c r="F98" s="25" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="G98" s="24"/>
       <c r="H98" s="24"/>
@@ -17716,10 +17699,10 @@
         <v>42</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="F99" s="25" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="G99" s="25"/>
       <c r="H99" s="24"/>
@@ -17733,7 +17716,7 @@
     </row>
     <row r="100" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A100" s="21" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B100" s="22"/>
       <c r="C100" s="23" t="s">
@@ -17746,7 +17729,7 @@
         <v>896</v>
       </c>
       <c r="F100" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G100" s="24"/>
       <c r="H100" s="24"/>
@@ -17768,10 +17751,10 @@
         <v>42</v>
       </c>
       <c r="E101" s="25" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="F101" s="25" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="G101" s="25"/>
       <c r="H101" s="24"/>
@@ -17785,7 +17768,7 @@
     </row>
     <row r="102" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A102" s="21" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B102" s="22"/>
       <c r="C102" s="23" t="s">
@@ -17798,7 +17781,7 @@
         <v>896</v>
       </c>
       <c r="F102" s="25" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="G102" s="24"/>
       <c r="H102" s="24"/>
@@ -17820,10 +17803,10 @@
         <v>42</v>
       </c>
       <c r="E103" s="25" t="s">
+        <v>1010</v>
+      </c>
+      <c r="F103" s="25" t="s">
         <v>1011</v>
-      </c>
-      <c r="F103" s="25" t="s">
-        <v>1012</v>
       </c>
       <c r="G103" s="25"/>
       <c r="H103" s="24"/>
@@ -17845,10 +17828,10 @@
         <v>42</v>
       </c>
       <c r="E104" s="25" t="s">
+        <v>1012</v>
+      </c>
+      <c r="F104" s="25" t="s">
         <v>1013</v>
-      </c>
-      <c r="F104" s="25" t="s">
-        <v>1014</v>
       </c>
       <c r="G104" s="25"/>
       <c r="H104" s="24"/>
@@ -17863,7 +17846,7 @@
     <row r="105" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A105" s="21"/>
       <c r="B105" s="22" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C105" s="23" t="s">
         <v>5</v>
@@ -17872,10 +17855,10 @@
         <v>42</v>
       </c>
       <c r="E105" s="25" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F105" s="25" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="G105" s="25"/>
       <c r="H105" s="24"/>
@@ -17897,10 +17880,10 @@
         <v>42</v>
       </c>
       <c r="E106" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F106" s="25" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="G106" s="25"/>
       <c r="H106" s="24"/>
@@ -17915,7 +17898,7 @@
     <row r="107" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A107" s="21"/>
       <c r="B107" s="22" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C107" s="23" t="s">
         <v>5</v>
@@ -17924,10 +17907,10 @@
         <v>42</v>
       </c>
       <c r="E107" s="25" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F107" s="25" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="G107" s="25"/>
       <c r="H107" s="24"/>
@@ -17949,10 +17932,10 @@
         <v>42</v>
       </c>
       <c r="E108" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F108" s="25" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="G108" s="25"/>
       <c r="H108" s="24"/>
@@ -17967,7 +17950,7 @@
     <row r="109" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A109" s="21"/>
       <c r="B109" s="59" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C109" s="23" t="s">
         <v>5</v>
@@ -17976,10 +17959,10 @@
         <v>42</v>
       </c>
       <c r="E109" s="25" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F109" s="25" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="G109" s="25"/>
       <c r="H109" s="24"/>
@@ -17994,7 +17977,7 @@
     <row r="110" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A110" s="21"/>
       <c r="B110" s="59" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C110" s="23" t="s">
         <v>5</v>
@@ -18003,10 +17986,10 @@
         <v>42</v>
       </c>
       <c r="E110" s="25" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F110" s="25" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="G110" s="25"/>
       <c r="H110" s="24"/>
@@ -18021,7 +18004,7 @@
     <row r="111" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A111" s="21"/>
       <c r="B111" s="22" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C111" s="23" t="s">
         <v>5</v>
@@ -18030,10 +18013,10 @@
         <v>42</v>
       </c>
       <c r="E111" s="25" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F111" s="25" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="G111" s="25"/>
       <c r="H111" s="24"/>
@@ -18060,7 +18043,7 @@
         <v>896</v>
       </c>
       <c r="F112" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G112" s="24"/>
       <c r="H112" s="24"/>
@@ -18085,7 +18068,7 @@
         <v>789</v>
       </c>
       <c r="F113" s="25" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="G113" s="24"/>
       <c r="H113" s="24"/>
@@ -18099,7 +18082,7 @@
     </row>
     <row r="114" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A114" s="21" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B114" s="22"/>
       <c r="C114" s="23" t="s">
@@ -18112,7 +18095,7 @@
         <v>896</v>
       </c>
       <c r="F114" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G114" s="24"/>
       <c r="H114" s="24"/>
@@ -18134,10 +18117,10 @@
         <v>42</v>
       </c>
       <c r="E115" s="25" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="F115" s="25" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="G115" s="6"/>
       <c r="H115" s="24"/>
@@ -18152,7 +18135,7 @@
     <row r="116" spans="1:15" s="2" customFormat="1" ht="105">
       <c r="A116" s="21"/>
       <c r="B116" s="22" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C116" s="23" t="s">
         <v>5</v>
@@ -18161,10 +18144,10 @@
         <v>42</v>
       </c>
       <c r="E116" s="25" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F116" s="25" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="G116" s="6"/>
       <c r="H116" s="24"/>
@@ -18178,7 +18161,7 @@
     </row>
     <row r="117" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A117" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B117" s="22"/>
       <c r="C117" s="23" t="s">
@@ -18191,7 +18174,7 @@
         <v>896</v>
       </c>
       <c r="F117" s="25" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="G117" s="24"/>
       <c r="H117" s="24"/>
@@ -18213,10 +18196,10 @@
         <v>42</v>
       </c>
       <c r="E118" s="25" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="F118" s="25" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="G118" s="6"/>
       <c r="H118" s="24"/>
@@ -18231,7 +18214,7 @@
     <row r="119" spans="1:15" s="2" customFormat="1" ht="105">
       <c r="A119" s="21"/>
       <c r="B119" s="22" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="C119" s="23" t="s">
         <v>5</v>
@@ -18240,10 +18223,10 @@
         <v>42</v>
       </c>
       <c r="E119" s="25" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="F119" s="25" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="G119" s="6"/>
       <c r="H119" s="24"/>
@@ -18257,7 +18240,7 @@
     </row>
     <row r="120" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A120" s="21" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B120" s="22"/>
       <c r="C120" s="23" t="s">
@@ -18270,7 +18253,7 @@
         <v>896</v>
       </c>
       <c r="F120" s="25" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="24"/>
@@ -18292,10 +18275,10 @@
         <v>42</v>
       </c>
       <c r="E121" s="25" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="F121" s="25" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="G121" s="24"/>
       <c r="H121" s="24"/>
@@ -18317,10 +18300,10 @@
         <v>42</v>
       </c>
       <c r="E122" s="25" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="F122" s="25" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="G122" s="6"/>
       <c r="H122" s="24"/>
@@ -18334,10 +18317,10 @@
     </row>
     <row r="123" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A123" s="21" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B123" s="22" t="s">
         <v>1030</v>
-      </c>
-      <c r="B123" s="22" t="s">
-        <v>1031</v>
       </c>
       <c r="C123" s="23" t="s">
         <v>5</v>
@@ -18349,7 +18332,7 @@
         <v>6</v>
       </c>
       <c r="F123" s="25" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="G123" s="24"/>
       <c r="H123" s="24"/>
@@ -18371,10 +18354,10 @@
         <v>42</v>
       </c>
       <c r="E124" s="25" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="F124" s="42" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="G124" s="6"/>
       <c r="H124" s="24"/>
@@ -18389,7 +18372,7 @@
     <row r="125" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A125" s="21"/>
       <c r="B125" s="22" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="C125" s="23" t="s">
         <v>5</v>
@@ -18401,7 +18384,7 @@
         <v>6</v>
       </c>
       <c r="F125" s="25" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="G125" s="24"/>
       <c r="H125" s="24"/>
@@ -18423,10 +18406,10 @@
         <v>42</v>
       </c>
       <c r="E126" s="25" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="F126" s="42" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="G126" s="6"/>
       <c r="H126" s="24"/>
@@ -18441,7 +18424,7 @@
     <row r="127" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A127" s="21"/>
       <c r="B127" s="22" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="C127" s="23" t="s">
         <v>5</v>
@@ -18453,7 +18436,7 @@
         <v>6</v>
       </c>
       <c r="F127" s="25" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="G127" s="24"/>
       <c r="H127" s="24"/>
@@ -18475,10 +18458,10 @@
         <v>42</v>
       </c>
       <c r="E128" s="25" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="F128" s="44" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="G128" s="6"/>
       <c r="H128" s="24"/>
@@ -18493,7 +18476,7 @@
     <row r="129" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A129" s="21"/>
       <c r="B129" s="22" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C129" s="23" t="s">
         <v>5</v>
@@ -18505,7 +18488,7 @@
         <v>6</v>
       </c>
       <c r="F129" s="25" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="G129" s="24"/>
       <c r="H129" s="24"/>
@@ -18527,10 +18510,10 @@
         <v>42</v>
       </c>
       <c r="E130" s="25" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="F130" s="44" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="G130" s="6"/>
       <c r="H130" s="24"/>
@@ -18552,10 +18535,10 @@
         <v>42</v>
       </c>
       <c r="E131" s="25" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="F131" s="44" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="G131" s="6"/>
       <c r="H131" s="24"/>
@@ -18582,7 +18565,7 @@
         <v>896</v>
       </c>
       <c r="F132" s="25" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="G132" s="24"/>
       <c r="H132" s="24"/>
@@ -18604,10 +18587,10 @@
         <v>42</v>
       </c>
       <c r="E133" s="25" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F133" s="25" t="s">
         <v>1039</v>
-      </c>
-      <c r="F133" s="25" t="s">
-        <v>1040</v>
       </c>
       <c r="G133" s="6"/>
       <c r="H133" s="24"/>
@@ -18621,7 +18604,7 @@
     </row>
     <row r="134" spans="1:15" s="2" customFormat="1" ht="90">
       <c r="A134" s="21" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B134" s="22"/>
       <c r="C134" s="23" t="s">
@@ -18634,7 +18617,7 @@
         <v>896</v>
       </c>
       <c r="F134" s="25" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="G134" s="24"/>
       <c r="H134" s="24"/>
@@ -18656,10 +18639,10 @@
         <v>42</v>
       </c>
       <c r="E135" s="25" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="F135" s="25" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="G135" s="6"/>
       <c r="H135" s="24"/>
@@ -18681,10 +18664,10 @@
         <v>42</v>
       </c>
       <c r="E136" s="25" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F136" s="25" t="s">
         <v>1043</v>
-      </c>
-      <c r="F136" s="25" t="s">
-        <v>1044</v>
       </c>
       <c r="G136" s="6"/>
       <c r="H136" s="24"/>
@@ -18698,7 +18681,7 @@
     </row>
     <row r="137" spans="1:15" s="2" customFormat="1" ht="409.5">
       <c r="A137" s="21" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B137" s="22"/>
       <c r="C137" s="23" t="s">
@@ -18708,10 +18691,10 @@
         <v>42</v>
       </c>
       <c r="E137" s="25" t="s">
+        <v>1045</v>
+      </c>
+      <c r="F137" s="25" t="s">
         <v>1046</v>
-      </c>
-      <c r="F137" s="25" t="s">
-        <v>1047</v>
       </c>
       <c r="G137" s="6"/>
       <c r="H137" s="24"/>
@@ -18733,10 +18716,10 @@
         <v>42</v>
       </c>
       <c r="E138" s="25" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F138" s="25" t="s">
         <v>1048</v>
-      </c>
-      <c r="F138" s="25" t="s">
-        <v>1049</v>
       </c>
       <c r="G138" s="6"/>
       <c r="H138" s="24"/>
@@ -18758,10 +18741,10 @@
         <v>42</v>
       </c>
       <c r="E139" s="25" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F139" s="25" t="s">
         <v>1050</v>
-      </c>
-      <c r="F139" s="25" t="s">
-        <v>1051</v>
       </c>
       <c r="G139" s="24"/>
       <c r="H139" s="24"/>
@@ -18775,10 +18758,10 @@
     </row>
     <row r="140" spans="1:15" s="2" customFormat="1" ht="60">
       <c r="A140" s="21" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="C140" s="23" t="s">
         <v>5</v>
@@ -18787,10 +18770,10 @@
         <v>352</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F140" s="25" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G140" s="24"/>
       <c r="H140" s="24"/>
@@ -18805,7 +18788,7 @@
     <row r="141" spans="1:15" ht="23.1" customHeight="1">
       <c r="A141" s="21"/>
       <c r="B141" s="22" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="C141" s="23" t="s">
         <v>17</v>
@@ -18817,7 +18800,7 @@
         <v>620</v>
       </c>
       <c r="F141" s="24" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G141" s="24"/>
       <c r="H141" s="24"/>
@@ -18832,7 +18815,7 @@
     <row r="142" spans="1:15" ht="90">
       <c r="A142" s="21"/>
       <c r="B142" s="62" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="C142" s="23" t="s">
         <v>5</v>
@@ -18841,7 +18824,7 @@
         <v>394</v>
       </c>
       <c r="E142" s="60" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="F142" s="24"/>
       <c r="G142" s="24"/>
@@ -18857,7 +18840,7 @@
     <row r="143" spans="1:15" ht="23.1" customHeight="1">
       <c r="A143" s="21"/>
       <c r="B143" s="22" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="C143" s="23" t="s">
         <v>5</v>
@@ -18866,7 +18849,7 @@
         <v>394</v>
       </c>
       <c r="E143" s="61" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="F143" s="24"/>
       <c r="G143" s="24"/>
@@ -18882,7 +18865,7 @@
     <row r="144" spans="1:15" ht="45">
       <c r="A144" s="21"/>
       <c r="B144" s="22" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C144" s="23" t="s">
         <v>5</v>
@@ -18891,10 +18874,10 @@
         <v>42</v>
       </c>
       <c r="E144" s="24" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="F144" s="60" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G144" s="24"/>
       <c r="H144" s="24"/>
@@ -18916,7 +18899,7 @@
         <v>229</v>
       </c>
       <c r="E145" s="64" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="F145" s="64" t="s">
         <v>749</v>

</xml_diff>